<commit_message>
save auxiliary excel files
</commit_message>
<xml_diff>
--- a/Prototypes/AgPasture/Comparison/OutputList.xlsx
+++ b/Prototypes/AgPasture/Comparison/OutputList.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="1037">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="1049">
   <si>
     <t>[Clock].Today as Date</t>
   </si>
@@ -3138,6 +3138,42 @@
   </si>
   <si>
     <t>SwardName as Sward.Name</t>
+  </si>
+  <si>
+    <t>Ryegrass.Height</t>
+  </si>
+  <si>
+    <t>Ryegrass.RootDepth</t>
+  </si>
+  <si>
+    <t>Height as Ryegrass.Height</t>
+  </si>
+  <si>
+    <t>rootDepth as Ryegrass.RootDepth</t>
+  </si>
+  <si>
+    <t>speciesHeight(1) as Ryegrass.Height</t>
+  </si>
+  <si>
+    <t>speciesRootDepth(1) as Ryegrass.RootDepth</t>
+  </si>
+  <si>
+    <t>[AgPasture].Height as Ryegrass.Height</t>
+  </si>
+  <si>
+    <t>[AgPasture].RootDepth as Ryegrass.RootDepth</t>
+  </si>
+  <si>
+    <t>[Sward].Ryegrass.Height as Ryegrass.Height</t>
+  </si>
+  <si>
+    <t>[Sward].Ryegrass.RootDepth as Ryegrass.RootDepth</t>
+  </si>
+  <si>
+    <t>[Ryegrass].Height as Ryegrass.Height</t>
+  </si>
+  <si>
+    <t>[Ryegrass].RootDepth as Ryegrass.RootDepth</t>
   </si>
 </sst>
 </file>
@@ -5346,13 +5382,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T102"/>
+  <dimension ref="A1:T104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="Q51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomRight" activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5373,12 +5409,18 @@
       <c r="I1" t="s">
         <v>849</v>
       </c>
+      <c r="L1" s="5"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H2" s="4"/>
       <c r="I2" t="s">
         <v>850</v>
       </c>
+      <c r="J2" s="5"/>
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="J4" s="2" t="s">
@@ -5487,19 +5529,19 @@
         <f t="shared" ref="H7:H62" si="5">IF(LEN(SUBSTITUTE(T7,$B7,""))&lt;LEN(T7),0,1)</f>
         <v>0</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="4" t="s">
         <v>1036</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="P7" t="s">
+      <c r="P7" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7" s="4" t="s">
         <v>170</v>
       </c>
       <c r="T7" t="s">
@@ -5589,10 +5631,10 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="4" t="s">
         <v>306</v>
       </c>
       <c r="N9" t="s">
@@ -7418,7 +7460,7 @@
         <v>0</v>
       </c>
       <c r="G45">
-        <f t="shared" ref="G45:G87" si="11">IF(LEN(SUBSTITUTE(R45,$B45,""))&lt;LEN(R45),0,1)</f>
+        <f t="shared" ref="G45:G89" si="11">IF(LEN(SUBSTITUTE(R45,$B45,""))&lt;LEN(R45),0,1)</f>
         <v>0</v>
       </c>
       <c r="H45">
@@ -8340,7 +8382,7 @@
         <v>0</v>
       </c>
       <c r="H63">
-        <f t="shared" ref="H63:H87" si="12">IF(LEN(SUBSTITUTE(T63,$B63,""))&lt;LEN(T63),0,1)</f>
+        <f t="shared" ref="H63:H89" si="12">IF(LEN(SUBSTITUTE(T63,$B63,""))&lt;LEN(T63),0,1)</f>
         <v>0</v>
       </c>
       <c r="J63" s="3" t="s">
@@ -8677,19 +8719,19 @@
         <v>740</v>
       </c>
       <c r="C70">
-        <f t="shared" ref="C70:C102" si="13">IF(LEN(SUBSTITUTE(J70,$B70,""))&lt;LEN(J70),0,1)</f>
+        <f t="shared" ref="C70:C104" si="13">IF(LEN(SUBSTITUTE(J70,$B70,""))&lt;LEN(J70),0,1)</f>
         <v>0</v>
       </c>
       <c r="D70">
-        <f t="shared" ref="D70:D87" si="14">IF(LEN(SUBSTITUTE(L70,$B70,""))&lt;LEN(L70),0,1)</f>
+        <f t="shared" ref="D70:D89" si="14">IF(LEN(SUBSTITUTE(L70,$B70,""))&lt;LEN(L70),0,1)</f>
         <v>0</v>
       </c>
       <c r="E70">
-        <f t="shared" ref="E70:E87" si="15">IF(LEN(SUBSTITUTE(N70,$B70,""))&lt;LEN(N70),0,1)</f>
+        <f t="shared" ref="E70:E89" si="15">IF(LEN(SUBSTITUTE(N70,$B70,""))&lt;LEN(N70),0,1)</f>
         <v>0</v>
       </c>
       <c r="F70">
-        <f t="shared" ref="F70:F87" si="16">IF(LEN(SUBSTITUTE(P70,$B70,""))&lt;LEN(P70),0,1)</f>
+        <f t="shared" ref="F70:F89" si="16">IF(LEN(SUBSTITUTE(P70,$B70,""))&lt;LEN(P70),0,1)</f>
         <v>0</v>
       </c>
       <c r="G70">
@@ -8772,7 +8814,7 @@
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72">
-        <f t="shared" ref="A72:A102" si="17">A71+1</f>
+        <f t="shared" ref="A72:A104" si="17">A71+1</f>
         <v>67</v>
       </c>
       <c r="B72" t="s">
@@ -9442,27 +9484,27 @@
         <v>754</v>
       </c>
       <c r="C85">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="C85:C91" si="18">IF(LEN(SUBSTITUTE(J85,$B85,""))&lt;LEN(J85),0,1)</f>
         <v>0</v>
       </c>
       <c r="D85">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="D85:D91" si="19">IF(LEN(SUBSTITUTE(L85,$B85,""))&lt;LEN(L85),0,1)</f>
         <v>0</v>
       </c>
       <c r="E85">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="E85:E91" si="20">IF(LEN(SUBSTITUTE(N85,$B85,""))&lt;LEN(N85),0,1)</f>
         <v>0</v>
       </c>
       <c r="F85">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="F85:F91" si="21">IF(LEN(SUBSTITUTE(P85,$B85,""))&lt;LEN(P85),0,1)</f>
         <v>0</v>
       </c>
       <c r="G85">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="G85:G91" si="22">IF(LEN(SUBSTITUTE(R85,$B85,""))&lt;LEN(R85),0,1)</f>
         <v>0</v>
       </c>
       <c r="H85">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="H85:H91" si="23">IF(LEN(SUBSTITUTE(T85,$B85,""))&lt;LEN(T85),0,1)</f>
         <v>0</v>
       </c>
       <c r="J85" s="4" t="s">
@@ -9493,27 +9535,27 @@
         <v>755</v>
       </c>
       <c r="C86">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="D86">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="E86">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="F86">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="G86">
-        <f t="shared" si="11"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="H86">
-        <f t="shared" si="12"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="J86" s="4" t="s">
@@ -9541,49 +9583,49 @@
         <v>82</v>
       </c>
       <c r="B87" t="s">
-        <v>756</v>
+        <v>1037</v>
       </c>
       <c r="C87">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="D87">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="E87">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="F87">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="G87">
-        <f t="shared" si="11"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="H87">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J87" s="3" t="s">
-        <v>838</v>
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="J87" s="4" t="s">
+        <v>1039</v>
       </c>
       <c r="L87" t="s">
-        <v>853</v>
-      </c>
-      <c r="N87" s="3" t="s">
-        <v>861</v>
-      </c>
-      <c r="P87" s="3" t="s">
-        <v>870</v>
+        <v>1041</v>
+      </c>
+      <c r="N87" s="4" t="s">
+        <v>1043</v>
+      </c>
+      <c r="P87" t="s">
+        <v>1045</v>
       </c>
       <c r="R87" t="s">
-        <v>870</v>
+        <v>1045</v>
       </c>
       <c r="T87" t="s">
-        <v>886</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.25">
@@ -9592,49 +9634,49 @@
         <v>83</v>
       </c>
       <c r="B88" t="s">
-        <v>757</v>
+        <v>1038</v>
       </c>
       <c r="C88">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="D88">
-        <f t="shared" ref="D88:D98" si="18">IF(LEN(SUBSTITUTE(L88,$B88,""))&lt;LEN(L88),0,1)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="E88">
-        <f t="shared" ref="E88:E98" si="19">IF(LEN(SUBSTITUTE(N88,$B88,""))&lt;LEN(N88),0,1)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="F88">
-        <f t="shared" ref="F88:F98" si="20">IF(LEN(SUBSTITUTE(P88,$B88,""))&lt;LEN(P88),0,1)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="G88">
-        <f t="shared" ref="G88:G98" si="21">IF(LEN(SUBSTITUTE(R88,$B88,""))&lt;LEN(R88),0,1)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="H88">
-        <f t="shared" ref="H88:H98" si="22">IF(LEN(SUBSTITUTE(T88,$B88,""))&lt;LEN(T88),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="J88" s="3" t="s">
-        <v>839</v>
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="J88" s="4" t="s">
+        <v>1040</v>
       </c>
       <c r="L88" t="s">
-        <v>854</v>
-      </c>
-      <c r="N88" s="3" t="s">
-        <v>862</v>
-      </c>
-      <c r="P88" s="3" t="s">
-        <v>871</v>
+        <v>1042</v>
+      </c>
+      <c r="N88" s="4" t="s">
+        <v>1044</v>
+      </c>
+      <c r="P88" t="s">
+        <v>1046</v>
       </c>
       <c r="R88" t="s">
-        <v>871</v>
+        <v>1046</v>
       </c>
       <c r="T88" t="s">
-        <v>887</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.25">
@@ -9643,49 +9685,49 @@
         <v>84</v>
       </c>
       <c r="B89" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="C89">
-        <f t="shared" ref="C89:C93" si="23">IF(LEN(SUBSTITUTE(J89,$B89,""))&lt;LEN(J89),0,1)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="D89">
-        <f t="shared" ref="D89:D93" si="24">IF(LEN(SUBSTITUTE(L89,$B89,""))&lt;LEN(L89),0,1)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="E89">
-        <f t="shared" ref="E89:E93" si="25">IF(LEN(SUBSTITUTE(N89,$B89,""))&lt;LEN(N89),0,1)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="F89">
-        <f t="shared" ref="F89:F93" si="26">IF(LEN(SUBSTITUTE(P89,$B89,""))&lt;LEN(P89),0,1)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="G89">
-        <f t="shared" ref="G89:G93" si="27">IF(LEN(SUBSTITUTE(R89,$B89,""))&lt;LEN(R89),0,1)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="H89">
-        <f t="shared" ref="H89:H93" si="28">IF(LEN(SUBSTITUTE(T89,$B89,""))&lt;LEN(T89),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="J89" s="4" t="s">
-        <v>840</v>
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="J89" s="3" t="s">
+        <v>838</v>
       </c>
       <c r="L89" t="s">
-        <v>855</v>
-      </c>
-      <c r="N89" t="s">
-        <v>863</v>
-      </c>
-      <c r="P89" t="s">
-        <v>872</v>
+        <v>853</v>
+      </c>
+      <c r="N89" s="3" t="s">
+        <v>861</v>
+      </c>
+      <c r="P89" s="3" t="s">
+        <v>870</v>
       </c>
       <c r="R89" t="s">
-        <v>879</v>
+        <v>870</v>
       </c>
       <c r="T89" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.25">
@@ -9694,49 +9736,49 @@
         <v>85</v>
       </c>
       <c r="B90" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="C90">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="H90">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D90">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="E90">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="F90">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="G90">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="H90">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="J90" s="4" t="s">
-        <v>841</v>
+      <c r="J90" s="3" t="s">
+        <v>839</v>
       </c>
       <c r="L90" t="s">
-        <v>381</v>
-      </c>
-      <c r="N90" t="s">
-        <v>73</v>
-      </c>
-      <c r="P90" t="s">
-        <v>155</v>
+        <v>854</v>
+      </c>
+      <c r="N90" s="3" t="s">
+        <v>862</v>
+      </c>
+      <c r="P90" s="3" t="s">
+        <v>871</v>
       </c>
       <c r="R90" t="s">
-        <v>155</v>
+        <v>871</v>
       </c>
       <c r="T90" t="s">
-        <v>271</v>
+        <v>887</v>
       </c>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.25">
@@ -9745,49 +9787,49 @@
         <v>86</v>
       </c>
       <c r="B91" t="s">
-        <v>1021</v>
+        <v>758</v>
       </c>
       <c r="C91">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="H91">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="D91">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="E91">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="F91">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="G91">
-        <f t="shared" si="27"/>
-        <v>0</v>
-      </c>
-      <c r="H91">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
       <c r="J91" s="4" t="s">
-        <v>1023</v>
+        <v>840</v>
       </c>
       <c r="L91" t="s">
-        <v>1024</v>
-      </c>
-      <c r="N91" t="s">
-        <v>1033</v>
+        <v>855</v>
+      </c>
+      <c r="N91" s="4" t="s">
+        <v>863</v>
       </c>
       <c r="P91" t="s">
-        <v>1025</v>
+        <v>872</v>
       </c>
       <c r="R91" t="s">
-        <v>1031</v>
+        <v>879</v>
       </c>
       <c r="T91" t="s">
-        <v>1029</v>
+        <v>888</v>
       </c>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.25">
@@ -9796,49 +9838,49 @@
         <v>87</v>
       </c>
       <c r="B92" t="s">
-        <v>1022</v>
+        <v>759</v>
       </c>
       <c r="C92">
-        <f t="shared" ref="C92" si="29">IF(LEN(SUBSTITUTE(J92,$B92,""))&lt;LEN(J92),0,1)</f>
+        <f t="shared" ref="C91:C95" si="24">IF(LEN(SUBSTITUTE(J92,$B92,""))&lt;LEN(J92),0,1)</f>
         <v>0</v>
       </c>
       <c r="D92">
-        <f t="shared" ref="D92" si="30">IF(LEN(SUBSTITUTE(L92,$B92,""))&lt;LEN(L92),0,1)</f>
+        <f t="shared" ref="D91:D95" si="25">IF(LEN(SUBSTITUTE(L92,$B92,""))&lt;LEN(L92),0,1)</f>
         <v>0</v>
       </c>
       <c r="E92">
-        <f t="shared" ref="E92" si="31">IF(LEN(SUBSTITUTE(N92,$B92,""))&lt;LEN(N92),0,1)</f>
+        <f t="shared" ref="E91:E95" si="26">IF(LEN(SUBSTITUTE(N92,$B92,""))&lt;LEN(N92),0,1)</f>
         <v>0</v>
       </c>
       <c r="F92">
-        <f t="shared" ref="F92" si="32">IF(LEN(SUBSTITUTE(P92,$B92,""))&lt;LEN(P92),0,1)</f>
+        <f t="shared" ref="F91:F95" si="27">IF(LEN(SUBSTITUTE(P92,$B92,""))&lt;LEN(P92),0,1)</f>
         <v>0</v>
       </c>
       <c r="G92">
-        <f t="shared" ref="G92" si="33">IF(LEN(SUBSTITUTE(R92,$B92,""))&lt;LEN(R92),0,1)</f>
+        <f t="shared" ref="G91:G95" si="28">IF(LEN(SUBSTITUTE(R92,$B92,""))&lt;LEN(R92),0,1)</f>
         <v>0</v>
       </c>
       <c r="H92">
-        <f t="shared" ref="H92" si="34">IF(LEN(SUBSTITUTE(T92,$B92,""))&lt;LEN(T92),0,1)</f>
+        <f t="shared" ref="H91:H95" si="29">IF(LEN(SUBSTITUTE(T92,$B92,""))&lt;LEN(T92),0,1)</f>
         <v>0</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>1026</v>
+        <v>841</v>
       </c>
       <c r="L92" t="s">
-        <v>1027</v>
+        <v>381</v>
       </c>
       <c r="N92" t="s">
-        <v>1034</v>
+        <v>73</v>
       </c>
       <c r="P92" t="s">
-        <v>1028</v>
+        <v>155</v>
       </c>
       <c r="R92" t="s">
-        <v>1032</v>
+        <v>155</v>
       </c>
       <c r="T92" t="s">
-        <v>1030</v>
+        <v>271</v>
       </c>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.25">
@@ -9847,49 +9889,49 @@
         <v>88</v>
       </c>
       <c r="B93" t="s">
-        <v>760</v>
+        <v>1021</v>
       </c>
       <c r="C93">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D93">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="E93">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="F93">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="G93">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="H93">
-        <f t="shared" si="28"/>
-        <v>0</v>
-      </c>
-      <c r="J93" s="3" t="s">
-        <v>842</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="J93" s="4" t="s">
+        <v>1023</v>
       </c>
       <c r="L93" t="s">
-        <v>856</v>
-      </c>
-      <c r="N93" s="3" t="s">
-        <v>864</v>
-      </c>
-      <c r="P93" s="3" t="s">
-        <v>873</v>
+        <v>1024</v>
+      </c>
+      <c r="N93" t="s">
+        <v>1033</v>
+      </c>
+      <c r="P93" t="s">
+        <v>1025</v>
       </c>
       <c r="R93" t="s">
-        <v>873</v>
+        <v>1031</v>
       </c>
       <c r="T93" t="s">
-        <v>889</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.25">
@@ -9898,49 +9940,49 @@
         <v>89</v>
       </c>
       <c r="B94" t="s">
-        <v>761</v>
+        <v>1022</v>
       </c>
       <c r="C94">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="C94" si="30">IF(LEN(SUBSTITUTE(J94,$B94,""))&lt;LEN(J94),0,1)</f>
         <v>0</v>
       </c>
       <c r="D94">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="D94" si="31">IF(LEN(SUBSTITUTE(L94,$B94,""))&lt;LEN(L94),0,1)</f>
         <v>0</v>
       </c>
       <c r="E94">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="E94" si="32">IF(LEN(SUBSTITUTE(N94,$B94,""))&lt;LEN(N94),0,1)</f>
         <v>0</v>
       </c>
       <c r="F94">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="F94" si="33">IF(LEN(SUBSTITUTE(P94,$B94,""))&lt;LEN(P94),0,1)</f>
         <v>0</v>
       </c>
       <c r="G94">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="G94" si="34">IF(LEN(SUBSTITUTE(R94,$B94,""))&lt;LEN(R94),0,1)</f>
         <v>0</v>
       </c>
       <c r="H94">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="H94" si="35">IF(LEN(SUBSTITUTE(T94,$B94,""))&lt;LEN(T94),0,1)</f>
         <v>0</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>843</v>
+        <v>1026</v>
       </c>
       <c r="L94" t="s">
-        <v>382</v>
+        <v>1027</v>
       </c>
       <c r="N94" t="s">
-        <v>74</v>
+        <v>1034</v>
       </c>
       <c r="P94" t="s">
-        <v>156</v>
+        <v>1028</v>
       </c>
       <c r="R94" t="s">
-        <v>880</v>
+        <v>1032</v>
       </c>
       <c r="T94" t="s">
-        <v>890</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.25">
@@ -9949,49 +9991,49 @@
         <v>90</v>
       </c>
       <c r="B95" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="C95">
-        <f t="shared" si="13"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D95">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="E95">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="F95">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="G95">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="H95">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="J95" s="4" t="s">
-        <v>844</v>
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="J95" s="3" t="s">
+        <v>842</v>
       </c>
       <c r="L95" t="s">
-        <v>383</v>
-      </c>
-      <c r="N95" t="s">
-        <v>75</v>
-      </c>
-      <c r="P95" t="s">
-        <v>157</v>
+        <v>856</v>
+      </c>
+      <c r="N95" s="3" t="s">
+        <v>864</v>
+      </c>
+      <c r="P95" s="3" t="s">
+        <v>873</v>
       </c>
       <c r="R95" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="T95" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.25">
@@ -10000,49 +10042,49 @@
         <v>91</v>
       </c>
       <c r="B96" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="C96">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D96">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="D90:D100" si="36">IF(LEN(SUBSTITUTE(L96,$B96,""))&lt;LEN(L96),0,1)</f>
         <v>0</v>
       </c>
       <c r="E96">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="E90:E100" si="37">IF(LEN(SUBSTITUTE(N96,$B96,""))&lt;LEN(N96),0,1)</f>
         <v>0</v>
       </c>
       <c r="F96">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="F90:F100" si="38">IF(LEN(SUBSTITUTE(P96,$B96,""))&lt;LEN(P96),0,1)</f>
         <v>0</v>
       </c>
       <c r="G96">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="G90:G100" si="39">IF(LEN(SUBSTITUTE(R96,$B96,""))&lt;LEN(R96),0,1)</f>
         <v>0</v>
       </c>
       <c r="H96">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="J96" t="s">
-        <v>845</v>
+        <f t="shared" ref="H90:H100" si="40">IF(LEN(SUBSTITUTE(T96,$B96,""))&lt;LEN(T96),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="J96" s="4" t="s">
+        <v>843</v>
       </c>
       <c r="L96" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="N96" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P96" t="s">
-        <v>874</v>
+        <v>156</v>
       </c>
       <c r="R96" t="s">
-        <v>874</v>
+        <v>880</v>
       </c>
       <c r="T96" t="s">
-        <v>272</v>
+        <v>890</v>
       </c>
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.25">
@@ -10051,49 +10093,49 @@
         <v>92</v>
       </c>
       <c r="B97" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="C97">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D97">
-        <f t="shared" si="18"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="E97">
-        <f t="shared" si="19"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="F97">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="G97">
-        <f t="shared" si="21"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="H97">
-        <f t="shared" si="22"/>
-        <v>0</v>
-      </c>
-      <c r="J97" s="3" t="s">
-        <v>846</v>
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="J97" s="4" t="s">
+        <v>844</v>
       </c>
       <c r="L97" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="N97" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P97" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="R97" t="s">
-        <v>158</v>
+        <v>881</v>
       </c>
       <c r="T97" t="s">
-        <v>273</v>
+        <v>891</v>
       </c>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.25">
@@ -10102,49 +10144,49 @@
         <v>93</v>
       </c>
       <c r="B98" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="C98">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D98">
-        <f t="shared" si="18"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="E98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="F98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="G98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="H98">
-        <f t="shared" si="22"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="J98" t="s">
-        <v>386</v>
+        <v>845</v>
       </c>
       <c r="L98" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="N98" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P98" t="s">
-        <v>159</v>
+        <v>874</v>
       </c>
       <c r="R98" t="s">
-        <v>159</v>
+        <v>874</v>
       </c>
       <c r="T98" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="99" spans="1:20" x14ac:dyDescent="0.25">
@@ -10153,49 +10195,49 @@
         <v>94</v>
       </c>
       <c r="B99" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="C99">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D99">
-        <f t="shared" ref="D99:D102" si="35">IF(LEN(SUBSTITUTE(L99,$B99,""))&lt;LEN(L99),0,1)</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="E99">
-        <f t="shared" ref="E99:E102" si="36">IF(LEN(SUBSTITUTE(N99,$B99,""))&lt;LEN(N99),0,1)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="F99">
-        <f t="shared" ref="F99:F102" si="37">IF(LEN(SUBSTITUTE(P99,$B99,""))&lt;LEN(P99),0,1)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="G99">
-        <f t="shared" ref="G99:G102" si="38">IF(LEN(SUBSTITUTE(R99,$B99,""))&lt;LEN(R99),0,1)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="H99">
-        <f t="shared" ref="H99:H102" si="39">IF(LEN(SUBSTITUTE(T99,$B99,""))&lt;LEN(T99),0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="J99" t="s">
-        <v>387</v>
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="J99" s="3" t="s">
+        <v>846</v>
       </c>
       <c r="L99" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="N99" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P99" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="R99" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="T99" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="100" spans="1:20" x14ac:dyDescent="0.25">
@@ -10204,49 +10246,49 @@
         <v>95</v>
       </c>
       <c r="B100" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="C100">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D100">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="E100">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="F100">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="G100">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="H100">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="J100" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="L100" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="N100" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P100" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="R100" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="T100" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="101" spans="1:20" x14ac:dyDescent="0.25">
@@ -10255,49 +10297,49 @@
         <v>96</v>
       </c>
       <c r="B101" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="C101">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D101">
-        <f t="shared" si="35"/>
+        <f t="shared" ref="D101:D104" si="41">IF(LEN(SUBSTITUTE(L101,$B101,""))&lt;LEN(L101),0,1)</f>
         <v>0</v>
       </c>
       <c r="E101">
-        <f t="shared" si="36"/>
+        <f t="shared" ref="E101:E104" si="42">IF(LEN(SUBSTITUTE(N101,$B101,""))&lt;LEN(N101),0,1)</f>
         <v>0</v>
       </c>
       <c r="F101">
-        <f t="shared" si="37"/>
+        <f t="shared" ref="F101:F104" si="43">IF(LEN(SUBSTITUTE(P101,$B101,""))&lt;LEN(P101),0,1)</f>
         <v>0</v>
       </c>
       <c r="G101">
-        <f t="shared" si="38"/>
+        <f t="shared" ref="G101:G104" si="44">IF(LEN(SUBSTITUTE(R101,$B101,""))&lt;LEN(R101),0,1)</f>
         <v>0</v>
       </c>
       <c r="H101">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="J101" s="4" t="s">
-        <v>389</v>
-      </c>
-      <c r="L101" s="5" t="s">
-        <v>858</v>
-      </c>
-      <c r="N101" s="4" t="s">
-        <v>164</v>
+        <f t="shared" ref="H101:H104" si="45">IF(LEN(SUBSTITUTE(T101,$B101,""))&lt;LEN(T101),0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="J101" t="s">
+        <v>387</v>
+      </c>
+      <c r="L101" t="s">
+        <v>387</v>
+      </c>
+      <c r="N101" t="s">
+        <v>79</v>
       </c>
       <c r="P101" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="R101" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="T101" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.25">
@@ -10306,69 +10348,171 @@
         <v>97</v>
       </c>
       <c r="B102" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="C102">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="D102">
-        <f t="shared" si="35"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="E102">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="F102">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="G102">
-        <f t="shared" si="38"/>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="H102">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="J102" s="4" t="s">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="J102" t="s">
+        <v>388</v>
+      </c>
+      <c r="L102" t="s">
+        <v>388</v>
+      </c>
+      <c r="N102" t="s">
+        <v>80</v>
+      </c>
+      <c r="P102" t="s">
+        <v>161</v>
+      </c>
+      <c r="R102" t="s">
+        <v>161</v>
+      </c>
+      <c r="T102" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <f t="shared" si="17"/>
+        <v>98</v>
+      </c>
+      <c r="B103" t="s">
+        <v>768</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="G103">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="J103" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="L103" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="N103" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="P103" t="s">
+        <v>162</v>
+      </c>
+      <c r="R103" t="s">
+        <v>162</v>
+      </c>
+      <c r="T103" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <f t="shared" si="17"/>
+        <v>99</v>
+      </c>
+      <c r="B104" t="s">
+        <v>769</v>
+      </c>
+      <c r="C104">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="G104">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="H104">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="J104" s="4" t="s">
         <v>847</v>
       </c>
-      <c r="L102" s="5" t="s">
+      <c r="L104" s="5" t="s">
         <v>857</v>
       </c>
-      <c r="N102" s="4" t="s">
+      <c r="N104" s="4" t="s">
         <v>865</v>
       </c>
-      <c r="P102" t="s">
+      <c r="P104" t="s">
         <v>875</v>
       </c>
-      <c r="R102" t="s">
+      <c r="R104" t="s">
         <v>875</v>
       </c>
-      <c r="T102" t="s">
+      <c r="T104" t="s">
         <v>892</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C6:F91 H6:H91 H93:H102 C93:F102">
+  <conditionalFormatting sqref="H95:H104 C95:F104 C6:F93 H6:H93">
     <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:G91 G93:G102">
+  <conditionalFormatting sqref="G95:G104 G6:G93">
     <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C92:F92 H92">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="C94:F94 H94">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G92">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="G94">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12714,12 +12858,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C6:F44 H6:H44">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6:G44">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>